<commit_message>
Lines of code for Add pet, Register sample_others test cases are updated
</commit_message>
<xml_diff>
--- a/animalBiome_Automation/src/test/resources/data/samples.xlsx
+++ b/animalBiome_Automation/src/test/resources/data/samples.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="5030" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14150" windowHeight="3400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SAMPLE_ID" sheetId="1" r:id="rId1"/>
     <sheet name="PET_NAME" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D11"/>
+  <oleSize ref="A1:D10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="267">
   <si>
     <t>User_Dog_Gut</t>
   </si>
@@ -771,9 +771,6 @@
     <t>KEF67M</t>
   </si>
   <si>
-    <t>scout1</t>
-  </si>
-  <si>
     <t>fury1</t>
   </si>
   <si>
@@ -783,7 +780,43 @@
     <t>Thunder2</t>
   </si>
   <si>
-    <t>Ryder2</t>
+    <t>Rabbit1</t>
+  </si>
+  <si>
+    <t>Cattle1</t>
+  </si>
+  <si>
+    <t>Sheep1</t>
+  </si>
+  <si>
+    <t>Primate2</t>
+  </si>
+  <si>
+    <t>Rabbit2</t>
+  </si>
+  <si>
+    <t>Cattle2</t>
+  </si>
+  <si>
+    <t>Bird3</t>
+  </si>
+  <si>
+    <t>Sheep2</t>
+  </si>
+  <si>
+    <t>Primate3</t>
+  </si>
+  <si>
+    <t>Rabbit3</t>
+  </si>
+  <si>
+    <t>Cattle3</t>
+  </si>
+  <si>
+    <t>Bird4</t>
+  </si>
+  <si>
+    <t>Sheep3</t>
   </si>
 </sst>
 </file>
@@ -837,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -856,6 +889,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
@@ -1164,7 +1204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1484,7 +1524,7 @@
       <c r="D17" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="20" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1501,7 +1541,7 @@
       <c r="D18" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="21" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1518,7 +1558,7 @@
       <c r="D19" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="22" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1535,7 +1575,7 @@
       <c r="D20" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="23" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1552,7 +1592,7 @@
       <c r="D21" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="24" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1569,7 +1609,7 @@
       <c r="D22" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="25" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1586,7 +1626,7 @@
       <c r="D23" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="26" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2034,10 +2074,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2085,6 +2125,9 @@
       <c r="C2" t="s" s="0">
         <v>30</v>
       </c>
+      <c r="D2" t="s" s="0">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
@@ -2093,26 +2136,64 @@
       <c r="C3" t="s" s="0">
         <v>30</v>
       </c>
+      <c r="D3" t="s" s="0">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C4" t="s" s="0">
-        <v>252</v>
+        <v>251</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C5" t="s" s="0">
-        <v>253</v>
+        <v>252</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C6" t="s" s="0">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35"/>
+        <v>253</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D7" t="s" s="0">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D8" t="s" s="0">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D9" t="s" s="0">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D10" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" t="s" s="0">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" t="s" s="0">
+        <v>266</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Lines of code for Add pet, Register sample_Dog test cases are updated
</commit_message>
<xml_diff>
--- a/animalBiome_Automation/src/test/resources/data/samples.xlsx
+++ b/animalBiome_Automation/src/test/resources/data/samples.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14150" windowHeight="3400" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14570" windowHeight="2760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SAMPLE_ID" sheetId="1" r:id="rId1"/>
     <sheet name="PET_NAME" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D10"/>
+  <oleSize ref="A10:D16"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="299">
   <si>
     <t>User_Dog_Gut</t>
   </si>
@@ -81,9 +81,6 @@
     <t>FGTHPA</t>
   </si>
   <si>
-    <t>GPHXPA</t>
-  </si>
-  <si>
     <t>M4CF4T</t>
   </si>
   <si>
@@ -789,27 +786,12 @@
     <t>Sheep1</t>
   </si>
   <si>
-    <t>Primate2</t>
-  </si>
-  <si>
-    <t>Rabbit2</t>
-  </si>
-  <si>
-    <t>Cattle2</t>
-  </si>
-  <si>
     <t>Bird3</t>
   </si>
   <si>
     <t>Sheep2</t>
   </si>
   <si>
-    <t>Primate3</t>
-  </si>
-  <si>
-    <t>Rabbit3</t>
-  </si>
-  <si>
     <t>Cattle3</t>
   </si>
   <si>
@@ -817,6 +799,120 @@
   </si>
   <si>
     <t>Sheep3</t>
+  </si>
+  <si>
+    <t>CKXFNF</t>
+  </si>
+  <si>
+    <t>EYERRG</t>
+  </si>
+  <si>
+    <t>F4XVUC</t>
+  </si>
+  <si>
+    <t>A6DECD</t>
+  </si>
+  <si>
+    <t>GFURHK</t>
+  </si>
+  <si>
+    <t>FGVJRH</t>
+  </si>
+  <si>
+    <t>URPPPY</t>
+  </si>
+  <si>
+    <t>67K3FX</t>
+  </si>
+  <si>
+    <t>GVHJEH</t>
+  </si>
+  <si>
+    <t>7A4DAX</t>
+  </si>
+  <si>
+    <t>4ENGMN</t>
+  </si>
+  <si>
+    <t>K3YKFX</t>
+  </si>
+  <si>
+    <t>YDRJYD</t>
+  </si>
+  <si>
+    <t>TDEDCT</t>
+  </si>
+  <si>
+    <t>KFMEXM</t>
+  </si>
+  <si>
+    <t>GN4XV9</t>
+  </si>
+  <si>
+    <t>ANHYXJ</t>
+  </si>
+  <si>
+    <t>DFN4MC</t>
+  </si>
+  <si>
+    <t>GMEUKV</t>
+  </si>
+  <si>
+    <t>REVUMK</t>
+  </si>
+  <si>
+    <t>MRMPHE</t>
+  </si>
+  <si>
+    <t>UFVUFY</t>
+  </si>
+  <si>
+    <t>4JRPUA</t>
+  </si>
+  <si>
+    <t>7VRCVX</t>
+  </si>
+  <si>
+    <t>CUXVMJ</t>
+  </si>
+  <si>
+    <t>GFGGJT</t>
+  </si>
+  <si>
+    <t>KVEDY9</t>
+  </si>
+  <si>
+    <t>VNF3UP</t>
+  </si>
+  <si>
+    <t>HRKETE</t>
+  </si>
+  <si>
+    <t>3DKJUC</t>
+  </si>
+  <si>
+    <t>Taffy1</t>
+  </si>
+  <si>
+    <t>Taffy2</t>
+  </si>
+  <si>
+    <t>Charlie4</t>
+  </si>
+  <si>
+    <t>Leo3</t>
+  </si>
+  <si>
+    <t>Snowy2</t>
+  </si>
+  <si>
+    <t>Milo3</t>
+  </si>
+  <si>
+    <t>Charlie5</t>
+  </si>
+  <si>
+    <t>Taffy3</t>
   </si>
 </sst>
 </file>
@@ -870,7 +966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -894,6 +990,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
@@ -1205,7 +1317,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1260,153 +1372,153 @@
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>101</v>
+      <c r="B2" s="31" t="s">
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>102</v>
+      <c r="B3" s="32" t="s">
+        <v>101</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="E7" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E10" s="13" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1414,16 +1526,16 @@
         <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -1431,16 +1543,16 @@
         <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -1448,16 +1560,16 @@
         <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1465,16 +1577,16 @@
         <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1482,16 +1594,16 @@
         <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1499,16 +1611,16 @@
         <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1516,16 +1628,16 @@
         <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1533,16 +1645,16 @@
         <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1550,16 +1662,16 @@
         <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1567,16 +1679,16 @@
         <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1584,16 +1696,16 @@
         <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1601,16 +1713,16 @@
         <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1618,16 +1730,16 @@
         <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1635,16 +1747,16 @@
         <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>48</v>
+        <v>222</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1652,16 +1764,16 @@
         <v>67</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>49</v>
+        <v>223</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1669,16 +1781,16 @@
         <v>68</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>50</v>
+        <v>224</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1686,13 +1798,16 @@
         <v>69</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1700,13 +1815,16 @@
         <v>70</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1714,13 +1832,16 @@
         <v>71</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1728,13 +1849,16 @@
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1742,13 +1866,16 @@
         <v>73</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1756,316 +1883,387 @@
         <v>74</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+        <v>230</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+        <v>231</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+        <v>232</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+        <v>241</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+        <v>242</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+        <v>247</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E52" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E53" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E54" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E55" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E56" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2076,8 +2274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2120,78 +2318,102 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>29</v>
+      </c>
       <c r="C4" t="s" s="0">
+        <v>250</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>251</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D5" t="s" s="0">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s" s="0">
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C5" t="s" s="0">
-        <v>252</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C6" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D7" t="s" s="0">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D8" t="s" s="0">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D12" t="s" s="0">
         <v>260</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D9" t="s" s="0">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D10" t="s" s="0">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="D11" t="s" s="0">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="D12" t="s" s="0">
-        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
My_Account(user profile)dog and Add pet, Register_sample_cat scenarios are committed.
</commit_message>
<xml_diff>
--- a/animalBiome_Automation/src/test/resources/data/samples.xlsx
+++ b/animalBiome_Automation/src/test/resources/data/samples.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14570" windowHeight="2760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14570" windowHeight="2870"/>
   </bookViews>
   <sheets>
     <sheet name="SAMPLE_ID" sheetId="1" r:id="rId1"/>
     <sheet name="PET_NAME" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A10:D16"/>
+  <oleSize ref="A16:G22"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="296">
   <si>
     <t>User_Dog_Gut</t>
   </si>
@@ -891,35 +891,25 @@
     <t>3DKJUC</t>
   </si>
   <si>
-    <t>Taffy1</t>
-  </si>
-  <si>
-    <t>Taffy2</t>
-  </si>
-  <si>
-    <t>Charlie4</t>
-  </si>
-  <si>
-    <t>Leo3</t>
-  </si>
-  <si>
-    <t>Snowy2</t>
-  </si>
-  <si>
-    <t>Milo3</t>
-  </si>
-  <si>
-    <t>Charlie5</t>
-  </si>
-  <si>
-    <t>Taffy3</t>
+    <t>Taffy4</t>
+  </si>
+  <si>
+    <t>Polo3</t>
+  </si>
+  <si>
+    <t>Kitty1</t>
+  </si>
+  <si>
+    <t>Onyx1</t>
+  </si>
+  <si>
+    <t>Cutie1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -936,7 +926,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -945,11 +935,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
         <fgColor indexed="13"/>
       </patternFill>
     </fill>
@@ -966,7 +951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1003,13 +988,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1314,26 +1306,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="17.81640625"/>
-    <col min="2" max="2" customWidth="true" style="1" width="15.0"/>
-    <col min="3" max="3" customWidth="true" style="1" width="15.36328125"/>
-    <col min="4" max="4" customWidth="true" style="1" width="17.453125"/>
-    <col min="5" max="5" customWidth="true" style="1" width="16.6328125"/>
-    <col min="6" max="6" customWidth="true" style="1" width="18.0"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.26953125"/>
-    <col min="8" max="8" customWidth="true" style="1" width="18.1796875"/>
-    <col min="9" max="9" customWidth="true" style="1" width="18.36328125"/>
-    <col min="10" max="10" customWidth="true" style="1" width="17.453125"/>
-    <col min="11" max="11" customWidth="true" style="1" width="17.36328125"/>
-    <col min="12" max="16384" style="1" width="8.7265625"/>
+    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.36328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.36328125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -1491,7 +1483,7 @@
       <c r="A9" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="45" t="s">
         <v>107</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1508,7 +1500,7 @@
       <c r="A10" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="48" t="s">
         <v>108</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1522,7 +1514,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="43" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1539,7 +1531,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="44" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1556,7 +1548,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="46" t="s">
         <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1573,7 +1565,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="47" t="s">
         <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1590,7 +1582,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="49" t="s">
         <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2274,145 +2266,136 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.90625"/>
-    <col min="2" max="2" customWidth="true" width="29.453125"/>
-    <col min="3" max="3" customWidth="true" width="35.6328125"/>
-    <col min="4" max="4" customWidth="true" width="30.90625"/>
-    <col min="5" max="5" customWidth="true" width="32.7265625"/>
-    <col min="6" max="6" customWidth="true" width="32.1796875"/>
-    <col min="7" max="7" customWidth="true" width="33.6328125"/>
-    <col min="8" max="8" customWidth="true" width="31.26953125"/>
+    <col min="1" max="1" width="26.90625" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="3" max="3" width="35.6328125" customWidth="1"/>
+    <col min="4" max="4" width="30.90625" customWidth="1"/>
+    <col min="5" max="5" width="32.7265625" customWidth="1"/>
+    <col min="6" max="6" width="32.1796875" customWidth="1"/>
+    <col min="7" max="7" width="33.6328125" customWidth="1"/>
+    <col min="8" max="8" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s" s="0">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s" s="0">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="B4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>250</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
-        <v>296</v>
-      </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>251</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>252</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>260</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed lines of code for add cat through sample registration.
</commit_message>
<xml_diff>
--- a/animalBiome_Automation/src/test/resources/data/samples.xlsx
+++ b/animalBiome_Automation/src/test/resources/data/samples.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14570" windowHeight="2870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14240" windowHeight="2530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SAMPLE_ID" sheetId="1" r:id="rId1"/>
     <sheet name="PET_NAME" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A16:G22"/>
+  <oleSize ref="A1:D7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="296">
   <si>
     <t>User_Dog_Gut</t>
   </si>
@@ -897,13 +897,13 @@
     <t>Polo3</t>
   </si>
   <si>
-    <t>Kitty1</t>
-  </si>
-  <si>
-    <t>Onyx1</t>
-  </si>
-  <si>
-    <t>Cutie1</t>
+    <t>Cutie3</t>
+  </si>
+  <si>
+    <t>Cinder3</t>
+  </si>
+  <si>
+    <t>Kitty3</t>
   </si>
 </sst>
 </file>
@@ -926,7 +926,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -936,6 +936,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -951,7 +957,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -999,6 +1005,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1308,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1367,10 +1378,10 @@
       <c r="B2" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="53" t="s">
         <v>200</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1384,10 +1395,10 @@
       <c r="B3" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="52" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="54" t="s">
         <v>201</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -1401,10 +1412,10 @@
       <c r="B4" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="51" t="s">
         <v>202</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1421,7 +1432,7 @@
       <c r="C5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="51" t="s">
         <v>203</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -2266,8 +2277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2313,7 +2324,7 @@
         <v>292</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -2327,7 +2338,7 @@
         <v>291</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -2341,7 +2352,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>295</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>250</v>
@@ -2354,14 +2365,17 @@
       <c r="A5" t="s">
         <v>29</v>
       </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
       <c r="C5" t="s">
-        <v>251</v>
-      </c>
-      <c r="D5" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>293</v>
+      </c>
       <c r="C6" t="s">
         <v>252</v>
       </c>
@@ -2370,11 +2384,20 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7" t="s">
+        <v>251</v>
+      </c>
       <c r="D7" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>295</v>
+      </c>
       <c r="D8" t="s">
         <v>256</v>
       </c>

</xml_diff>

<commit_message>
Lines of code updated for cat and horse test cases
</commit_message>
<xml_diff>
--- a/animalBiome_Automation/src/test/resources/data/samples.xlsx
+++ b/animalBiome_Automation/src/test/resources/data/samples.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14240" windowHeight="2530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14240" windowHeight="2680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SAMPLE_ID" sheetId="1" r:id="rId1"/>
     <sheet name="PET_NAME" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D7"/>
+  <oleSize ref="A4:D10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="308">
   <si>
     <t>User_Dog_Gut</t>
   </si>
@@ -618,18 +618,6 @@
     <t>PATJTJ</t>
   </si>
   <si>
-    <t>R4JHYN</t>
-  </si>
-  <si>
-    <t>TNPCEU</t>
-  </si>
-  <si>
-    <t>CFDGCU</t>
-  </si>
-  <si>
-    <t>NJFJTH</t>
-  </si>
-  <si>
     <t>XAN6GY</t>
   </si>
   <si>
@@ -891,25 +879,74 @@
     <t>3DKJUC</t>
   </si>
   <si>
-    <t>Taffy4</t>
-  </si>
-  <si>
-    <t>Polo3</t>
-  </si>
-  <si>
-    <t>Cutie3</t>
-  </si>
-  <si>
-    <t>Cinder3</t>
-  </si>
-  <si>
-    <t>Kitty3</t>
+    <t>Taffy6</t>
+  </si>
+  <si>
+    <t>Taffy7</t>
+  </si>
+  <si>
+    <t>Taffy8</t>
+  </si>
+  <si>
+    <t>Charlie7</t>
+  </si>
+  <si>
+    <t>Leo5</t>
+  </si>
+  <si>
+    <t>Snowy5</t>
+  </si>
+  <si>
+    <t>Milo6</t>
+  </si>
+  <si>
+    <t>Polo4</t>
+  </si>
+  <si>
+    <t>Onyx6</t>
+  </si>
+  <si>
+    <t>Cutie5</t>
+  </si>
+  <si>
+    <t>Cinder5</t>
+  </si>
+  <si>
+    <t>Kitty5</t>
+  </si>
+  <si>
+    <t>scout2</t>
+  </si>
+  <si>
+    <t>fury2</t>
+  </si>
+  <si>
+    <t>Bandit2</t>
+  </si>
+  <si>
+    <t>Thunder3</t>
+  </si>
+  <si>
+    <t>Primate4</t>
+  </si>
+  <si>
+    <t>Primate5</t>
+  </si>
+  <si>
+    <t>Rabbit4</t>
+  </si>
+  <si>
+    <t>Cattle4</t>
+  </si>
+  <si>
+    <t>Bird5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -939,9 +976,8 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
   </fills>
@@ -957,7 +993,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1009,10 +1045,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1317,26 +1370,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.36328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.36328125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="17.81640625"/>
+    <col min="2" max="2" customWidth="true" style="1" width="15.0"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.36328125"/>
+    <col min="4" max="4" customWidth="true" style="1" width="17.453125"/>
+    <col min="5" max="5" customWidth="true" style="1" width="16.6328125"/>
+    <col min="6" max="6" customWidth="true" style="1" width="18.0"/>
+    <col min="7" max="7" customWidth="true" style="1" width="17.26953125"/>
+    <col min="8" max="8" customWidth="true" style="1" width="18.1796875"/>
+    <col min="9" max="9" customWidth="true" style="1" width="18.36328125"/>
+    <col min="10" max="10" customWidth="true" style="1" width="17.453125"/>
+    <col min="11" max="11" customWidth="true" style="1" width="17.36328125"/>
+    <col min="12" max="16384" style="1" width="8.7265625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -1381,7 +1434,7 @@
       <c r="C2" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="58" t="s">
         <v>200</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1395,10 +1448,10 @@
       <c r="B3" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="60" t="s">
         <v>201</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -1412,10 +1465,10 @@
       <c r="B4" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="1" t="s">
         <v>202</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1429,10 +1482,10 @@
       <c r="B5" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="1" t="s">
         <v>203</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -1446,7 +1499,7 @@
       <c r="B6" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="54" t="s">
         <v>154</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1463,7 +1516,7 @@
       <c r="B7" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="55" t="s">
         <v>155</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1480,7 +1533,7 @@
       <c r="B8" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="56" t="s">
         <v>156</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1497,7 +1550,7 @@
       <c r="B9" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="57" t="s">
         <v>157</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1514,7 +1567,7 @@
       <c r="B10" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="59" t="s">
         <v>158</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1531,7 +1584,7 @@
       <c r="B11" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="61" t="s">
         <v>159</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1548,7 +1601,7 @@
       <c r="B12" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="62" t="s">
         <v>160</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1565,7 +1618,7 @@
       <c r="B13" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="63" t="s">
         <v>161</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1582,7 +1635,7 @@
       <c r="B14" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="64" t="s">
         <v>162</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1599,7 +1652,7 @@
       <c r="B15" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="65" t="s">
         <v>163</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1610,13 +1663,13 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="71" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="66" t="s">
         <v>164</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1633,7 +1686,7 @@
       <c r="B17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="67" t="s">
         <v>165</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1650,7 +1703,7 @@
       <c r="B18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="68" t="s">
         <v>166</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1667,7 +1720,7 @@
       <c r="B19" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="69" t="s">
         <v>167</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1684,7 +1737,7 @@
       <c r="B20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="70" t="s">
         <v>168</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1810,7 +1863,7 @@
         <v>225</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1827,7 +1880,7 @@
         <v>226</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1844,7 +1897,7 @@
         <v>227</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1861,7 +1914,7 @@
         <v>228</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1878,7 +1931,7 @@
         <v>229</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1895,7 +1948,7 @@
         <v>230</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1912,7 +1965,7 @@
         <v>231</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1929,7 +1982,7 @@
         <v>232</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1946,7 +1999,7 @@
         <v>233</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1963,7 +2016,7 @@
         <v>234</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1980,7 +2033,7 @@
         <v>235</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1997,7 +2050,7 @@
         <v>236</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -2014,7 +2067,7 @@
         <v>237</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -2031,7 +2084,7 @@
         <v>238</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -2048,7 +2101,7 @@
         <v>239</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -2065,7 +2118,7 @@
         <v>240</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -2082,7 +2135,7 @@
         <v>241</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -2099,7 +2152,7 @@
         <v>242</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -2116,7 +2169,7 @@
         <v>243</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -2133,7 +2186,7 @@
         <v>244</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -2150,7 +2203,7 @@
         <v>245</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -2163,11 +2216,8 @@
       <c r="C48" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>246</v>
-      </c>
       <c r="E48" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
@@ -2180,11 +2230,8 @@
       <c r="C49" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>247</v>
-      </c>
       <c r="E49" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
@@ -2197,11 +2244,8 @@
       <c r="C50" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="E50" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -2214,11 +2258,8 @@
       <c r="C51" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="E51" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
@@ -2226,7 +2267,7 @@
         <v>94</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
@@ -2234,7 +2275,7 @@
         <v>95</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
@@ -2242,7 +2283,7 @@
         <v>96</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
@@ -2250,7 +2291,7 @@
         <v>97</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
@@ -2258,7 +2299,7 @@
         <v>98</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
@@ -2275,151 +2316,177 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.90625" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" customWidth="1"/>
-    <col min="3" max="3" width="35.6328125" customWidth="1"/>
-    <col min="4" max="4" width="30.90625" customWidth="1"/>
-    <col min="5" max="5" width="32.7265625" customWidth="1"/>
-    <col min="6" max="6" width="32.1796875" customWidth="1"/>
-    <col min="7" max="7" width="33.6328125" customWidth="1"/>
-    <col min="8" max="8" width="31.26953125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="26.90625"/>
+    <col min="2" max="2" customWidth="true" width="29.453125"/>
+    <col min="3" max="3" customWidth="true" width="35.6328125"/>
+    <col min="4" max="4" customWidth="true" width="30.90625"/>
+    <col min="5" max="5" customWidth="true" width="32.7265625"/>
+    <col min="6" max="6" customWidth="true" width="32.1796875"/>
+    <col min="7" max="7" customWidth="true" width="33.6328125"/>
+    <col min="8" max="8" customWidth="true" width="31.26953125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
+        <v>290</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>288</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>300</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>289</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>249</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
         <v>292</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" t="s" s="0">
+        <v>248</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="B7" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C7" t="s" s="0">
+        <v>247</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="B8" t="s" s="0">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>291</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C8" t="s" s="0">
+        <v>301</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>250</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C9" t="s" s="0">
+        <v>302</v>
+      </c>
+      <c r="D9" t="s" s="0">
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>293</v>
-      </c>
-      <c r="C6" t="s">
-        <v>252</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D10" t="s" s="0">
         <v>254</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>294</v>
-      </c>
-      <c r="C7" t="s">
-        <v>251</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D11" t="s" s="0">
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>295</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D12" t="s" s="0">
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D9" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D10" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D11" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D12" t="s">
-        <v>260</v>
+    <row r="13">
+      <c r="D13" t="s" s="0">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for User_Others view all reports,share pet profile scenarios
</commit_message>
<xml_diff>
--- a/animalBiome_Automation/src/test/resources/data/samples.xlsx
+++ b/animalBiome_Automation/src/test/resources/data/samples.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14240" windowHeight="2680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14410" windowHeight="2000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SAMPLE_ID" sheetId="1" r:id="rId1"/>
     <sheet name="PET_NAME" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A4:D10"/>
+  <oleSize ref="B10:E14"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="312">
   <si>
     <t>User_Dog_Gut</t>
   </si>
@@ -768,27 +768,6 @@
     <t>Rabbit1</t>
   </si>
   <si>
-    <t>Cattle1</t>
-  </si>
-  <si>
-    <t>Sheep1</t>
-  </si>
-  <si>
-    <t>Bird3</t>
-  </si>
-  <si>
-    <t>Sheep2</t>
-  </si>
-  <si>
-    <t>Cattle3</t>
-  </si>
-  <si>
-    <t>Bird4</t>
-  </si>
-  <si>
-    <t>Sheep3</t>
-  </si>
-  <si>
     <t>CKXFNF</t>
   </si>
   <si>
@@ -879,67 +858,100 @@
     <t>3DKJUC</t>
   </si>
   <si>
-    <t>Taffy6</t>
-  </si>
-  <si>
-    <t>Taffy7</t>
-  </si>
-  <si>
-    <t>Taffy8</t>
-  </si>
-  <si>
-    <t>Charlie7</t>
-  </si>
-  <si>
-    <t>Leo5</t>
-  </si>
-  <si>
-    <t>Snowy5</t>
-  </si>
-  <si>
-    <t>Milo6</t>
-  </si>
-  <si>
-    <t>Polo4</t>
-  </si>
-  <si>
-    <t>Onyx6</t>
-  </si>
-  <si>
-    <t>Cutie5</t>
-  </si>
-  <si>
-    <t>Cinder5</t>
-  </si>
-  <si>
-    <t>Kitty5</t>
-  </si>
-  <si>
-    <t>scout2</t>
-  </si>
-  <si>
-    <t>fury2</t>
-  </si>
-  <si>
-    <t>Bandit2</t>
-  </si>
-  <si>
     <t>Thunder3</t>
   </si>
   <si>
-    <t>Primate4</t>
-  </si>
-  <si>
-    <t>Primate5</t>
-  </si>
-  <si>
-    <t>Rabbit4</t>
-  </si>
-  <si>
-    <t>Cattle4</t>
-  </si>
-  <si>
-    <t>Bird5</t>
+    <t>Kitty6</t>
+  </si>
+  <si>
+    <t>Leo7</t>
+  </si>
+  <si>
+    <t>Snowy7</t>
+  </si>
+  <si>
+    <t>Milo8</t>
+  </si>
+  <si>
+    <t>Kitty7</t>
+  </si>
+  <si>
+    <t>pony3</t>
+  </si>
+  <si>
+    <t>scout3</t>
+  </si>
+  <si>
+    <t>fury3</t>
+  </si>
+  <si>
+    <t>Bandit3</t>
+  </si>
+  <si>
+    <t>Thunder4</t>
+  </si>
+  <si>
+    <t>Ryder3</t>
+  </si>
+  <si>
+    <t>Charlie10</t>
+  </si>
+  <si>
+    <t>Leo8</t>
+  </si>
+  <si>
+    <t>Snowy8</t>
+  </si>
+  <si>
+    <t>Milo9</t>
+  </si>
+  <si>
+    <t>Taffy13</t>
+  </si>
+  <si>
+    <t>Polo8</t>
+  </si>
+  <si>
+    <t>Kitty8</t>
+  </si>
+  <si>
+    <t>pony4</t>
+  </si>
+  <si>
+    <t>Cattle8</t>
+  </si>
+  <si>
+    <t>Primate12</t>
+  </si>
+  <si>
+    <t>Rabbit11</t>
+  </si>
+  <si>
+    <t>Cattle9</t>
+  </si>
+  <si>
+    <t>Bird10</t>
+  </si>
+  <si>
+    <t>Sheep10</t>
+  </si>
+  <si>
+    <t>Charlie11</t>
+  </si>
+  <si>
+    <t>Charlie12</t>
+  </si>
+  <si>
+    <t>Leo9</t>
+  </si>
+  <si>
+    <t>Snowy9</t>
+  </si>
+  <si>
+    <t>Milo10</t>
+  </si>
+  <si>
+    <t>Taffy14</t>
   </si>
 </sst>
 </file>
@@ -993,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1065,6 +1077,58 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1372,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1468,7 +1532,7 @@
       <c r="C4" s="52" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="79" t="s">
         <v>202</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1485,7 +1549,7 @@
       <c r="C5" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="80" t="s">
         <v>203</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -1502,7 +1566,7 @@
       <c r="C6" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="81" t="s">
         <v>204</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -1519,7 +1583,7 @@
       <c r="C7" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="101" t="s">
         <v>205</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -1536,7 +1600,7 @@
       <c r="C8" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="102" t="s">
         <v>206</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -1553,7 +1617,7 @@
       <c r="C9" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="111" t="s">
         <v>207</v>
       </c>
       <c r="E9" s="12" t="s">
@@ -1570,7 +1634,7 @@
       <c r="C10" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="112" t="s">
         <v>208</v>
       </c>
       <c r="E10" s="13" t="s">
@@ -1581,7 +1645,7 @@
       <c r="A11" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="73" t="s">
         <v>109</v>
       </c>
       <c r="C11" s="61" t="s">
@@ -1598,7 +1662,7 @@
       <c r="A12" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="99" t="s">
         <v>110</v>
       </c>
       <c r="C12" s="62" t="s">
@@ -1615,7 +1679,7 @@
       <c r="A13" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="108" t="s">
         <v>111</v>
       </c>
       <c r="C13" s="63" t="s">
@@ -1680,7 +1744,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="72" t="s">
         <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1697,7 +1761,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="74" t="s">
         <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1714,7 +1778,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="95" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1731,7 +1795,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="96" t="s">
         <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1748,13 +1812,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="97" t="s">
         <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="75" t="s">
         <v>169</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1765,13 +1829,13 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="98" t="s">
         <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="76" t="s">
         <v>170</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1782,13 +1846,13 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="107" t="s">
         <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="77" t="s">
         <v>171</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1799,13 +1863,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="109" t="s">
         <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="78" t="s">
         <v>172</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1822,7 +1886,7 @@
       <c r="B25" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="100" t="s">
         <v>173</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1839,7 +1903,7 @@
       <c r="B26" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="110" t="s">
         <v>174</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -1862,8 +1926,8 @@
       <c r="D27" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>257</v>
+      <c r="E27" s="82" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1879,8 +1943,8 @@
       <c r="D28" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>258</v>
+      <c r="E28" s="83" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1896,8 +1960,8 @@
       <c r="D29" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>259</v>
+      <c r="E29" s="84" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1913,8 +1977,8 @@
       <c r="D30" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>260</v>
+      <c r="E30" s="85" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1930,8 +1994,8 @@
       <c r="D31" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>261</v>
+      <c r="E31" s="86" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1947,8 +2011,8 @@
       <c r="D32" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>262</v>
+      <c r="E32" s="87" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1964,8 +2028,8 @@
       <c r="D33" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>263</v>
+      <c r="E33" s="88" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1981,8 +2045,8 @@
       <c r="D34" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>264</v>
+      <c r="E34" s="89" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1998,8 +2062,8 @@
       <c r="D35" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>265</v>
+      <c r="E35" s="90" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -2015,8 +2079,8 @@
       <c r="D36" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>266</v>
+      <c r="E36" s="91" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -2032,8 +2096,8 @@
       <c r="D37" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>267</v>
+      <c r="E37" s="92" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -2049,8 +2113,8 @@
       <c r="D38" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>268</v>
+      <c r="E38" s="93" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -2066,8 +2130,8 @@
       <c r="D39" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>269</v>
+      <c r="E39" s="94" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -2083,8 +2147,8 @@
       <c r="D40" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>270</v>
+      <c r="E40" s="103" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -2100,8 +2164,8 @@
       <c r="D41" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>271</v>
+      <c r="E41" s="104" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -2117,8 +2181,8 @@
       <c r="D42" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>272</v>
+      <c r="E42" s="105" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -2134,8 +2198,8 @@
       <c r="D43" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>273</v>
+      <c r="E43" s="106" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -2151,8 +2215,8 @@
       <c r="D44" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>274</v>
+      <c r="E44" s="113" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -2168,8 +2232,8 @@
       <c r="D45" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>275</v>
+      <c r="E45" s="114" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -2185,8 +2249,8 @@
       <c r="D46" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>276</v>
+      <c r="E46" s="115" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -2202,8 +2266,8 @@
       <c r="D47" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>277</v>
+      <c r="E47" s="116" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -2216,8 +2280,8 @@
       <c r="C48" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>278</v>
+      <c r="E48" s="117" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
@@ -2230,8 +2294,8 @@
       <c r="C49" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>279</v>
+      <c r="E49" s="118" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
@@ -2244,8 +2308,8 @@
       <c r="C50" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>280</v>
+      <c r="E50" s="119" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -2258,32 +2322,32 @@
       <c r="C51" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>281</v>
+      <c r="E51" s="120" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>282</v>
+      <c r="E52" s="121" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>283</v>
+      <c r="E53" s="122" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>284</v>
+      <c r="E54" s="123" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
@@ -2291,7 +2355,7 @@
         <v>97</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
@@ -2299,7 +2363,7 @@
         <v>98</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
@@ -2316,10 +2380,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2362,133 +2426,178 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>295</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>299</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>303</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>296</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>300</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>304</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>297</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>246</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>305</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>249</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>306</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>29</v>
+        <v>286</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>248</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>250</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>29</v>
+        <v>298</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>247</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>251</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
+        <v>281</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>280</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>293</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>287</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s" s="0">
         <v>294</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>301</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B9" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D10" t="s" s="0">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C11" t="s" s="0">
+        <v>288</v>
+      </c>
       <c r="D11" t="s" s="0">
-        <v>255</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s" s="0">
+        <v>295</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>289</v>
+      </c>
       <c r="D12" t="s" s="0">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="D13" t="s" s="0">
-        <v>307</v>
-      </c>
-    </row>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s" s="0">
+        <v>308</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s" s="0">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s" s="0">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s" s="0">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>